<commit_message>
revision of some controlled vocs in excel and csv
</commit_message>
<xml_diff>
--- a/VocabolariControllati/TipiEventiPubblici/EventiPubblici_AllineamentoSchemaOrg.xlsx
+++ b/VocabolariControllati/TipiEventiPubblici/EventiPubblici_AllineamentoSchemaOrg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EventiPubblici.csv" sheetId="1" r:id="rId1"/>
@@ -19,37 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
-  <si>
-    <t>1.1 Mostra</t>
-  </si>
-  <si>
-    <t>1.3 Seminario / Conferenza /Workshop / Webinar / Simposio</t>
-  </si>
-  <si>
-    <t>1.5 Spettacolo teatrale</t>
-  </si>
-  <si>
-    <t>1.6 Spettacolo di danza</t>
-  </si>
-  <si>
-    <t>1.9 Festival</t>
-  </si>
-  <si>
-    <t>2. Evento Sportivo</t>
-  </si>
-  <si>
-    <t>3. Evento sociale</t>
-  </si>
-  <si>
-    <t>6. Evento di affari-commerciale</t>
-  </si>
-  <si>
-    <t>6.6 Mercato / Mercatino</t>
-  </si>
-  <si>
-    <t>7. Evento musicale</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Classificazione eventi pubblici</t>
   </si>
@@ -81,9 +51,6 @@
     <t>http://schema.org/VisualArtsEvent</t>
   </si>
   <si>
-    <t>1.2 Presentazione Libro</t>
-  </si>
-  <si>
     <t>http://schema.org/LiteraryEvent</t>
   </si>
   <si>
@@ -99,30 +66,18 @@
     <t>http://schema.org/DanceEvent</t>
   </si>
   <si>
-    <t>1.7 Proiezione Cinematografica</t>
-  </si>
-  <si>
     <t>http://schema.org/ComedyEvent</t>
   </si>
   <si>
     <t>http://schema.org/Festival</t>
   </si>
   <si>
-    <t>1,12 Corso</t>
-  </si>
-  <si>
     <t>http://schema.org/CourseInstance</t>
   </si>
   <si>
-    <t>6.1 Meeting d'affati</t>
-  </si>
-  <si>
     <t>http://schema.org/DeliveryEvent</t>
   </si>
   <si>
-    <t>6.4 Fiera / Salone</t>
-  </si>
-  <si>
     <t>http://schema.org/ExhibitionEvent</t>
   </si>
   <si>
@@ -132,13 +87,100 @@
     <t>http://schema.org/FoodEvent</t>
   </si>
   <si>
-    <t>3 Evento sociale</t>
-  </si>
-  <si>
     <t>http://schema.org/ChildrenEvent</t>
   </si>
   <si>
     <t>http://schema.org/ScreeningEvent</t>
+  </si>
+  <si>
+    <t>Codice tipo evento pubblico</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Evento Sportivo</t>
+  </si>
+  <si>
+    <t>Evento sociale</t>
+  </si>
+  <si>
+    <t>Evento di affari-commerciale</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>Evento musicale</t>
+  </si>
+  <si>
+    <t>Mostra</t>
+  </si>
+  <si>
+    <t>Presentazione Libro</t>
+  </si>
+  <si>
+    <t>Seminario / Conferenza /Workshop / Webinar / Simposio</t>
+  </si>
+  <si>
+    <t>Spettacolo teatrale</t>
+  </si>
+  <si>
+    <t>Spettacolo di danza</t>
+  </si>
+  <si>
+    <t>Proiezione Cinematografica</t>
+  </si>
+  <si>
+    <t>Festival</t>
+  </si>
+  <si>
+    <t>Corso</t>
+  </si>
+  <si>
+    <t>Meeting d'affati</t>
+  </si>
+  <si>
+    <t>Fiera / Salone</t>
+  </si>
+  <si>
+    <t>Mercato / Mercatino</t>
   </si>
 </sst>
 </file>
@@ -253,8 +295,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -630,340 +672,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="71.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="5">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="11" spans="1:4" ht="30">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30">
+      <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="30">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45">
-      <c r="A10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30">
-      <c r="A13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30">
-      <c r="A14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30">
-      <c r="A18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="5"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="5"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="5"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="5"/>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="5"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="5"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="5"/>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="5"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="5"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="5"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="5"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="5"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="5"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="5"/>
+    <row r="21" spans="1:4">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A39"/>
-    <mergeCell ref="A40:A45"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C14" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D14" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>